<commit_message>
PCB review / changement non pas ajuster
</commit_message>
<xml_diff>
--- a/Documentation/PCB/Plan_de_test/plan_de_tests_PCB_Connexion.xlsx
+++ b/Documentation/PCB/Plan_de_test/plan_de_tests_PCB_Connexion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programme\_TSO\_Projet tso final\Trotinette_Git\Documentation\PCB\Plan_de_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC8DAC-7E50-439E-B7D6-415B908DF7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8C77A8-51DF-4B99-AB76-71A1C992B0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
   </bookViews>
@@ -87,15 +87,6 @@
     <t>Est-ce que la chip sur l'écran pour activé le touch est présente?</t>
   </si>
   <si>
-    <t>Est-ce qu'elle s'insert bien dans les pin header femelle?</t>
-  </si>
-  <si>
-    <t>Insérer l'écran sur le PCB de connexion, connecter le port mini-HDMI à celui du PCB de télémétrie. Brancher le port USB-C du PCB de télémétrie pour alimenter le tout. Mettre le programme &lt;&lt;Accelerometre&gt;&gt; du git dans le MCU à l'aide de plateforme.io. Est-ce que l'écran affiche les angles ?</t>
-  </si>
-  <si>
-    <t>En gardant le branchement mentionné plus haut, est-ce que lorsqu'on touche l'écran, il est affiché à l'écran.</t>
-  </si>
-  <si>
     <t>La tension d'entrée est à 5V</t>
   </si>
   <si>
@@ -112,6 +103,15 @@
   </si>
   <si>
     <t>Marc-Antoine Sauvé</t>
+  </si>
+  <si>
+    <t>Est-ce que l'écran s'insert bien dans les pin header femelle?</t>
+  </si>
+  <si>
+    <t>Insérer l'écran sur le PCB de connexion, connecter le port mini-HDMI du PCB de connexion à celui du PCB de télémétrie. Brancher le port USB-C du PCB de télémétrie pour alimenter le tout. Mettre le programme &lt;&lt;Accelerometre&gt;&gt; du git dans le MCU à l'aide de plateforme.io. Est-ce que l'écran affiche les angles ?</t>
+  </si>
+  <si>
+    <t>En gardant le branchement mentionné plus haut ainsi que le code, est-ce que lorsqu'on touche l'écran, il est affiché à l'écran.</t>
   </si>
 </sst>
 </file>
@@ -190,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -199,8 +199,48 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF085C4D"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF085C4D"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF085C4D"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF085C4D"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF085C4D"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF085C4D"/>
       </left>
       <right/>
       <top/>
@@ -209,55 +249,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF085C4D"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FF085C4D"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF085C4D"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF085C4D"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF085C4D"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF085C4D"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thick">
         <color rgb="FF085C4D"/>
       </right>
@@ -374,54 +365,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="dashDot">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -431,48 +382,6 @@
       </right>
       <top/>
       <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="dashDotDot">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dashDotDot">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDotDot">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -497,15 +406,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -516,11 +476,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -529,97 +488,83 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,10 +803,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44BF1BC0-4CC6-4C5E-B5BA-D603BE4F90F0}" name="Table2" displayName="Table2" ref="B29:E38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44BF1BC0-4CC6-4C5E-B5BA-D603BE4F90F0}" name="Table2" displayName="Table2" ref="B22:E31" headerRowCount="0" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1F4C9926-DE17-4526-B1BD-9D183A491E88}" name="1" headerRowDxfId="9" dataDxfId="8">
-      <calculatedColumnFormula>B29+1</calculatedColumnFormula>
+      <calculatedColumnFormula>B22+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{E4B78305-54C7-43BC-B765-D086A3BDB66E}" name="Column1" headerRowDxfId="7" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{1D24A92F-EACA-4F96-AB25-C42E4D7DE336}" name="Column2" headerRowDxfId="5" dataDxfId="4"/>
@@ -1168,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A179C3DD-CE59-450A-90EC-B70C1216426A}">
-  <dimension ref="B1:G42"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,7 +1130,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2"/>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3"/>
@@ -1193,12 +1138,12 @@
     </row>
     <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5"/>
-      <c r="C2" s="46"/>
+      <c r="C2" s="42"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:7" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
-      <c r="C3" s="47"/>
+      <c r="C3" s="43"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1212,7 +1157,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -1220,7 +1165,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1243,7 +1188,7 @@
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="24">
         <v>1</v>
       </c>
       <c r="D7" s="8"/>
@@ -1258,278 +1203,236 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="27"/>
+      <c r="C11" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="27"/>
+      <c r="C12" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
+      <c r="C13" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="38"/>
-      <c r="C11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="38"/>
-      <c r="C12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="39"/>
-      <c r="C13" s="25" t="s">
+      <c r="D13" s="37"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="29"/>
+      <c r="C15" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="40"/>
-      <c r="C15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="14"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="B16" s="40"/>
-      <c r="C16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="21"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="40"/>
-      <c r="C17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="14"/>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="29"/>
+      <c r="C17" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="40"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="21"/>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="25"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="40"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="14"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="21"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="40"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="14"/>
+    <row r="21" spans="1:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="21"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="40"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="14"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="22">
+        <f t="shared" ref="B23:B30" si="0">B22+1</f>
+        <v>2</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="43"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="22">
+        <f>B23+1</f>
+        <v>3</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="44"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34">
-        <v>1</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="34">
-        <f t="shared" ref="B30:B37" si="0">B29+1</f>
-        <v>2</v>
-      </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="34">
-        <f>B30+1</f>
-        <v>3</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="34">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="34">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="22">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="34">
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="22">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="34">
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="22">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="34">
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="22">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="34">
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="22">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="34">
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="22">
         <v>10</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E39" s="35"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="35"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E41" s="35"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E42" s="35"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="23"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="23"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B24:B25"/>
+  <mergeCells count="2">
+    <mergeCell ref="B21:E21"/>
     <mergeCell ref="C1:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="D10:D25">
+  <conditionalFormatting sqref="D10:D18">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Échec">
       <formula>NOT(ISERROR(SEARCH("Échec",D10)))</formula>
     </cfRule>
@@ -1537,8 +1440,8 @@
       <formula>NOT(ISERROR(SEARCH("Réussi",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D25" xr:uid="{FE4B82E2-1996-4D3C-82E2-B8CCB3918355}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D18" xr:uid="{FE4B82E2-1996-4D3C-82E2-B8CCB3918355}">
       <formula1>$G$7:$G$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>